<commit_message>
Update attendance calculation logic and improve file structure
- Modified `AttendanceCalculator` to count meetings with at least 2 real participants.
- Updated average participants calculation to reflect the new meeting validation criteria.
- Changed input and output file paths in `main.py` for better organization.
- Revised README to clarify input/output directory structure and meeting validation rules.
- Adjusted attendance report outputs to reflect the updated calculations.
</commit_message>
<xml_diff>
--- a/output/attendance_report_september_2025.xlsx
+++ b/output/attendance_report_september_2025.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,7 +435,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="31" customWidth="1" min="1" max="1"/>
-    <col width="29" customWidth="1" min="2" max="2"/>
+    <col width="27" customWidth="1" min="2" max="2"/>
     <col width="19" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
@@ -480,13 +480,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E2" t="n">
-        <v>90.91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -501,13 +501,13 @@
         </is>
       </c>
       <c r="C3" t="n">
+        <v>17</v>
+      </c>
+      <c r="D3" t="n">
         <v>18</v>
       </c>
-      <c r="D3" t="n">
-        <v>22</v>
-      </c>
       <c r="E3" t="n">
-        <v>81.81999999999999</v>
+        <v>94.44</v>
       </c>
     </row>
     <row r="4">
@@ -525,10 +525,10 @@
         <v>16</v>
       </c>
       <c r="D4" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E4" t="n">
-        <v>72.73</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="5">
@@ -543,55 +543,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E5" t="n">
-        <v>68.18000000000001</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Muhammad Fuaad Zameer</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>fuaad.zameer@arbisoft.com</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>22</v>
-      </c>
-      <c r="E6" t="n">
-        <v>4.55</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Shafqat Farhan</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>shafqat.farhan@arbisoft.com</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>22</v>
-      </c>
-      <c r="E7" t="n">
-        <v>4.55</v>
+        <v>77.78</v>
       </c>
     </row>
   </sheetData>
@@ -636,7 +594,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
@@ -646,7 +604,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -657,7 +615,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>53.79%</t>
+          <t>90.28%</t>
         </is>
       </c>
     </row>
@@ -668,7 +626,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.23</v>
+        <v>3.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>